<commit_message>
Fix row height calculation (#5)
</commit_message>
<xml_diff>
--- a/src/ExcelsiorAspose.Tests/Tests.Render.verified.xlsx
+++ b/src/ExcelsiorAspose.Tests/Tests.Render.verified.xlsx
@@ -43,7 +43,7 @@
     <t>John Doe</t>
   </si>
   <si>
-    <t>📧 john@company.com</t>
+    <t>✉ john@company.com</t>
   </si>
   <si>
     <t>✓ Active</t>
@@ -55,13 +55,13 @@
     <t>Jane Smith</t>
   </si>
   <si>
-    <t>📧 jane@company.com</t>
+    <t>✉ jane@company.com</t>
   </si>
   <si>
     <t>Bob Johnson</t>
   </si>
   <si>
-    <t>📧 bob@company.com</t>
+    <t>✉ bob@company.com</t>
   </si>
   <si>
     <t>✗ Inactive</t>
@@ -73,7 +73,7 @@
     <t>Alice Brown</t>
   </si>
   <si>
-    <t>📧 alice@company.com</t>
+    <t>✉ alice@company.com</t>
   </si>
   <si>
     <t>Contract</t>
@@ -527,7 +527,7 @@
   <cols>
     <col min="1" max="1" width="14.7142857142857" customWidth="1"/>
     <col min="2" max="2" width="12.7142857142857" customWidth="1"/>
-    <col min="3" max="3" width="21.7142857142857" customWidth="1"/>
+    <col min="3" max="3" width="20.7142857142857" customWidth="1"/>
     <col min="4" max="4" width="11.7142857142857" customWidth="1"/>
     <col min="5" max="5" width="15.7142857142857" customWidth="1"/>
     <col min="6" max="6" width="10.7142857142857" customWidth="1"/>
@@ -626,7 +626,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="12.75">
+    <row r="5" spans="1:7" ht="13" customHeight="1">
       <c r="A5" s="1">
         <v>4</v>
       </c>

</xml_diff>

<commit_message>
fix ConvertToExtensionBlock doesnt work properly in net9 yet
</commit_message>
<xml_diff>
--- a/src/ExcelsiorAspose.Tests/Tests.Render.verified.xlsx
+++ b/src/ExcelsiorAspose.Tests/Tests.Render.verified.xlsx
@@ -40,10 +40,10 @@
     <t>Status</t>
   </si>
   <si>
-    <t>John Doe</t>
-  </si>
-  <si>
-    <t>✉ john@company.com</t>
+    <t>JOHN DOE</t>
+  </si>
+  <si>
+    <t>john@company.com</t>
   </si>
   <si>
     <t>✓ Active</t>
@@ -52,16 +52,16 @@
     <t>Full Time</t>
   </si>
   <si>
-    <t>Jane Smith</t>
-  </si>
-  <si>
-    <t>✉ jane@company.com</t>
-  </si>
-  <si>
-    <t>Bob Johnson</t>
-  </si>
-  <si>
-    <t>✉ bob@company.com</t>
+    <t>JANE SMITH</t>
+  </si>
+  <si>
+    <t>jane@company.com</t>
+  </si>
+  <si>
+    <t>BOB JOHNSON</t>
+  </si>
+  <si>
+    <t>bob@company.com</t>
   </si>
   <si>
     <t>✗ Inactive</t>
@@ -70,10 +70,10 @@
     <t>Part Time</t>
   </si>
   <si>
-    <t>Alice Brown</t>
-  </si>
-  <si>
-    <t>✉ alice@company.com</t>
+    <t>ALICE BROWN</t>
+  </si>
+  <si>
+    <t>alice@company.com</t>
   </si>
   <si>
     <t>Contract</t>
@@ -525,9 +525,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="14.7142857142857" customWidth="1"/>
-    <col min="2" max="2" width="12.7142857142857" customWidth="1"/>
-    <col min="3" max="3" width="20.7142857142857" customWidth="1"/>
+    <col min="1" max="2" width="14.7142857142857" customWidth="1"/>
+    <col min="3" max="3" width="18.7142857142857" customWidth="1"/>
     <col min="4" max="4" width="11.7142857142857" customWidth="1"/>
     <col min="5" max="5" width="15.7142857142857" customWidth="1"/>
     <col min="6" max="6" width="10.7142857142857" customWidth="1"/>

</xml_diff>